<commit_message>
modify the spreadsheet productos.xlsx to automatically generate the necessary SQL commands to insert the data into the tbproductos table
</commit_message>
<xml_diff>
--- a/archivos-excel/productos.xlsx
+++ b/archivos-excel/productos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Google Drive\03. Alura Latam\01. PRODUÇÃO\01. Cursos\A_ESP-Yoney Gallardo\1790 - Introducción a SQL con MySQL_ manipule y consulte datos\docs\1790 - Introducción a SQL con MySQL - Roteiro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayxa\Desktop\Web Development\ONE\SQL\archivos-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69DC3DE-681B-4F76-B04C-30DAA8CD4BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="productos" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">productos!$A$1:$D$36</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>SKU</t>
   </si>
@@ -153,12 +162,24 @@
   </si>
   <si>
     <t>ENVASE</t>
+  </si>
+  <si>
+    <t>QUERY</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>VOLUMEN</t>
+  </si>
+  <si>
+    <t>SABOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,21 +525,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +553,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>773912</v>
       </c>
@@ -545,8 +579,24 @@
       <c r="D2" s="1">
         <v>8.0079999999999991</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(" '",LEFT(B2,FIND(" -",B2,1)-1),"', ")</f>
+        <v xml:space="preserve"> 'Clean', </v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT("'",SUBSTITUTE(MID(SUBSTITUTE(" - " &amp;B2&amp;REPT(" ",6)," - ",REPT(",",255)),2*255,255),",",""),"', ")</f>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT("'",TRIM(RIGHT(SUBSTITUTE(B2," ",REPT(" ",100)),100)),"', ")</f>
+        <v xml:space="preserve">'Naranja', </v>
+      </c>
+      <c r="J2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (",A2,", ",F2,"'",C2,"', ", G2,H2,D2, ");")</f>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (773912,  'Clean', 'Botella PET', '1 Litro', 'Naranja', 8.008);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>838819</v>
       </c>
@@ -559,8 +609,24 @@
       <c r="D3" s="1">
         <v>12.007999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F36" si="0">_xlfn.CONCAT(" '",LEFT(B3,FIND(" -",B3,1)-1),"', ")</f>
+        <v xml:space="preserve"> 'Clean', </v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G36" si="1">_xlfn.CONCAT("'",SUBSTITUTE(MID(SUBSTITUTE(" - " &amp;B3&amp;REPT(" ",6)," - ",REPT(",",255)),2*255,255),",",""),"', ")</f>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H36" si="2">_xlfn.CONCAT("'",TRIM(RIGHT(SUBSTITUTE(B3," ",REPT(" ",100)),100)),"', ")</f>
+        <v xml:space="preserve">'Naranja', </v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J36" si="3">_xlfn.CONCAT("INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (",A3,", ",F3,"'",C3,"', ", G3,H3,D3, ");")</f>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (838819,  'Clean', 'Botella PET', '15 Litros', 'Naranja', 12.008);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1037797</v>
       </c>
@@ -573,8 +639,24 @@
       <c r="D4" s="1">
         <v>16.007999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Clean', </v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'2 Litros', </v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Naranja', </v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1037797,  'Clean', 'Botella PET', '2 Litros', 'Naranja', 16.008);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>812829</v>
       </c>
@@ -587,8 +669,24 @@
       <c r="D5" s="1">
         <v>2.8080000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Clean', </v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Naranja', </v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (812829,  'Clean', 'Lata', '350 ml', 'Naranja', 2.808);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>479745</v>
       </c>
@@ -601,8 +699,24 @@
       <c r="D6" s="1">
         <v>3.7680000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Clean', </v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'470 ml', </v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Naranja', </v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (479745,  'Clean', 'Botella de Vidrio', '470 ml', 'Naranja', 3.768);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>695594</v>
       </c>
@@ -615,8 +729,24 @@
       <c r="D7" s="1">
         <v>28.511999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Festival de Sabores', </v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Asaí', </v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (695594,  'Festival de Sabores', 'Botella PET', '15 Litros', 'Asaí', 28.512);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>243083</v>
       </c>
@@ -629,8 +759,24 @@
       <c r="D8" s="1">
         <v>10.512</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Festival de Sabores', </v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Maracuyá', </v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (243083,  'Festival de Sabores', 'Botella PET', '15 Litros', 'Maracuyá', 10.512);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1022450</v>
       </c>
@@ -643,8 +789,24 @@
       <c r="D9" s="1">
         <v>38.012</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Festival de Sabores', </v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'2 Litros', </v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Asái', </v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1022450,  'Festival de Sabores', 'Botella PET', '2 Litros', 'Asái', 38.012);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>231776</v>
       </c>
@@ -657,8 +819,24 @@
       <c r="D10" s="1">
         <v>13.312000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Festival de Sabores', </v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Asaí', </v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (231776,  'Festival de Sabores', 'Botella de Vidrio', '700 ml', 'Asaí', 13.312);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>723457</v>
       </c>
@@ -671,8 +849,24 @@
       <c r="D11" s="1">
         <v>4.911999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Festival de Sabores', </v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Maracuyá', </v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (723457,  'Festival de Sabores', 'Botella de Vidrio', '700 ml', 'Maracuyá', 4.912);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>746596</v>
       </c>
@@ -685,8 +879,24 @@
       <c r="D12" s="1">
         <v>19.504999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Light', </v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Sandía', </v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (746596,  'Light', 'Botella PET', '15 Litros', 'Sandía', 19.505);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1040107</v>
       </c>
@@ -699,8 +909,24 @@
       <c r="D13" s="1">
         <v>4.5549999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Light', </v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Sandía', </v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1040107,  'Light', 'Lata', '350 ml', 'Sandía', 4.555);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1002334</v>
       </c>
@@ -713,8 +939,24 @@
       <c r="D14" s="1">
         <v>7.0039999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Línea Citrus', </v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Lima/Limón', </v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1002334,  'Línea Citrus', 'Botella PET', '1 Litro', 'Lima/Limón', 7.004);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1041119</v>
       </c>
@@ -727,8 +969,24 @@
       <c r="D15" s="1">
         <v>4.903999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Línea Citrus', </v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Lima/Limón', </v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1041119,  'Línea Citrus', 'Botella de Vidrio', '700 ml', 'Lima/Limón', 4.904);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1088126</v>
       </c>
@@ -741,8 +999,24 @@
       <c r="D16" s="1">
         <v>7.0039999999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Línea Citrus', </v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Limón', </v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1088126,  'Línea Citrus', 'Botella PET', '1 Litro', 'Limón', 7.004);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1042712</v>
       </c>
@@ -755,8 +1029,24 @@
       <c r="D17" s="1">
         <v>4.903999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Línea Citrus', </v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Limón', </v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1042712,  'Línea Citrus', 'Botella de Vidrio', '700 ml', 'Limón', 4.904);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>520380</v>
       </c>
@@ -769,8 +1059,24 @@
       <c r="D18" s="1">
         <v>12.010999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Pedazos de Frutas', </v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Manzana', </v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (520380,  'Pedazos de Frutas', 'Botella PET', '1 Litro', 'Manzana', 12.011);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>788975</v>
       </c>
@@ -783,8 +1089,24 @@
       <c r="D19" s="1">
         <v>18.010999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Pedazos de Frutas', </v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Manzana', </v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (788975,  'Pedazos de Frutas', 'Botella PET', '15 Litros', 'Manzana', 18.011);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>229900</v>
       </c>
@@ -797,8 +1119,24 @@
       <c r="D20" s="1">
         <v>4.2110000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Pedazos de Frutas', </v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Manzana', </v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (229900,  'Pedazos de Frutas', 'Lata', '350 ml', 'Manzana', 4.211);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1086543</v>
       </c>
@@ -811,8 +1149,24 @@
       <c r="D21" s="1">
         <v>11.0105</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Refrescante', </v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Mango', </v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1086543,  'Refrescante', 'Botella PET', '1 Litro', 'Mango', 11.0105);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1101035</v>
       </c>
@@ -825,8 +1179,24 @@
       <c r="D22" s="1">
         <v>9.0105000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Refrescante', </v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'1 Litro', </v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Frutilla/Limón', </v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1101035,  'Refrescante', 'Botella PET', '1 Litro', 'Frutilla/Limón', 9.0105);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>326779</v>
       </c>
@@ -839,8 +1209,24 @@
       <c r="D23" s="1">
         <v>16.5105</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Refrescante', </v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Mango', </v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (326779,  'Refrescante', 'Botella PET', '15 Litros', 'Mango', 16.5105);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1096818</v>
       </c>
@@ -853,8 +1239,24 @@
       <c r="D24" s="1">
         <v>7.7105000000000006</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Refrescante', </v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Mango', </v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1096818,  'Refrescante', 'Botella de Vidrio', '700 ml', 'Mango', 7.7105);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>826490</v>
       </c>
@@ -867,8 +1269,24 @@
       <c r="D25" s="1">
         <v>6.3104999999999993</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Refrescante', </v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Frutilla/Limón', </v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (826490,  'Refrescante', 'Botella de Vidrio', '700 ml', 'Frutilla/Limón', 6.3105);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>394479</v>
       </c>
@@ -881,8 +1299,24 @@
       <c r="D26" s="1">
         <v>8.4089999999999989</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Sabor da Montaña', </v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Cereza', </v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (394479,  'Sabor da Montaña', 'Botella de Vidrio', '700 ml', 'Cereza', 8.409);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>783663</v>
       </c>
@@ -895,8 +1329,24 @@
       <c r="D27" s="1">
         <v>7.7090000000000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Sabor da Montaña', </v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Frutilla', </v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (783663,  'Sabor da Montaña', 'Botella de Vidrio', '700 ml', 'Frutilla', 7.709);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1000889</v>
       </c>
@@ -909,8 +1359,24 @@
       <c r="D28" s="1">
         <v>6.3090000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Sabor da Montaña', </v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Uva', </v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1000889,  'Sabor da Montaña', 'Botella de Vidrio', '700 ml', 'Uva', 6.309);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>544931</v>
       </c>
@@ -923,8 +1389,24 @@
       <c r="D29" s="1">
         <v>2.4594999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Verano', </v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Limón', </v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (544931,  'Verano', 'Lata', '350 ml', 'Limón', 2.4595);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>235653</v>
       </c>
@@ -937,8 +1419,24 @@
       <c r="D30" s="1">
         <v>3.8595000000000006</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Verano', </v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Mango', </v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (235653,  'Verano', 'Lata', '350 ml', 'Mango', 3.8595);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1051518</v>
       </c>
@@ -951,8 +1449,24 @@
       <c r="D31" s="1">
         <v>3.2995000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Verano', </v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'470 ml', </v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Limón', </v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1051518,  'Verano', 'Botella de Vidrio', '470 ml', 'Limón', 3.2995);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1078680</v>
       </c>
@@ -965,8 +1479,24 @@
       <c r="D32" s="1">
         <v>5.1795000000000009</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Verano', </v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'470 ml', </v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Mango', </v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1078680,  'Verano', 'Botella de Vidrio', '470 ml', 'Mango', 5.1795);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1004327</v>
       </c>
@@ -979,8 +1509,24 @@
       <c r="D33" s="1">
         <v>19.510000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Vida del Campo', </v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'15 Litros', </v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Sandía', </v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1004327,  'Vida del Campo', 'Botella PET', '15 Litros', 'Sandía', 19.51);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1002767</v>
       </c>
@@ -993,8 +1539,24 @@
       <c r="D34" s="1">
         <v>8.41</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Vida del Campo', </v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'700 ml', </v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Cereza/Manzana', </v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1002767,  'Vida del Campo', 'Botella de Vidrio', '700 ml', 'Cereza/Manzana', 8.41);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1013793</v>
       </c>
@@ -1007,8 +1569,24 @@
       <c r="D35" s="1">
         <v>24.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Vida del Campo', </v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'2 Litros', </v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Cereza/Manzana', </v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (1013793,  'Vida del Campo', 'Botella PET', '2 Litros', 'Cereza/Manzana', 24.01);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>290478</v>
       </c>
@@ -1020,6 +1598,22 @@
       </c>
       <c r="D36" s="1">
         <v>4.5599999999999996</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 'Vida del Campo', </v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">'350 ml', </v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">'Sandía', </v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `tbproductos`(producto, nombre, envase, volumen, sabor, precio) VALUES (290478,  'Vida del Campo', 'Lata', '350 ml', 'Sandía', 4.56);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>